<commit_message>
Update Motivation's Status , Effect'Status
</commit_message>
<xml_diff>
--- a/Assets/Scripts/1.Abilities/Resources/Documents/CombineAbilities/CombineAbililties_Motivation.xlsx
+++ b/Assets/Scripts/1.Abilities/Resources/Documents/CombineAbilities/CombineAbililties_Motivation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\BackUp 2023-0324\Unity Portfolios\BoilerPlate\BP\Assets\Scripts\1.Abilities\Resources\Documents\CombineAbilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\myWorks\Unity-BolierPlate-Codes\Assets\Scripts\1.Abilities\Resources\Documents\CombineAbilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC2F0E0-F3EF-4DB1-A912-1B5A8F8480D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449EDF87-684A-47D6-B5D0-DFA42D5DE66D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10410" yWindow="6120" windowWidth="24900" windowHeight="11860" activeTab="1" xr2:uid="{D49C7B43-6E4D-49C2-B7A8-3A3FDB66E59A}"/>
+    <workbookView xWindow="3495" yWindow="3495" windowWidth="28800" windowHeight="15345" xr2:uid="{D49C7B43-6E4D-49C2-B7A8-3A3FDB66E59A}"/>
   </bookViews>
   <sheets>
     <sheet name="AreaMotivatedAbility" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -82,6 +82,10 @@
   </si>
   <si>
     <t>MotivatedStatName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HasReflectMaxStatus</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -449,15 +453,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F5BC70-149D-4DE7-ACDA-32783B69FAC3}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,125 +469,128 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="1"/>
       <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L2" s="1"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L3" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L4" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L5" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L6" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L7" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L8" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L9" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L10" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L11" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L12" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L13" s="1"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L14" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L15" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="M5:O5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -592,15 +599,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA059A84-6AF1-4A91-9346-3006E82BB928}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -608,125 +615,128 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="1"/>
       <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L2" s="1"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L3" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L4" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L5" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L6" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L7" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L8" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L9" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L10" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L11" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L12" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L13" s="1"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L14" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L15" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="M5:O5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>